<commit_message>
update phan cong 2
</commit_message>
<xml_diff>
--- a/Do_An/Phân Công.xlsx
+++ b/Do_An/Phân Công.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tai lieu HK V\Android\DA_Android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tai lieu HK V\Android\Thunder_Team\Do_An\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -172,14 +172,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +464,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -484,10 +484,10 @@
       <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -511,7 +511,7 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="11">
         <v>9</v>
       </c>
     </row>
@@ -529,7 +529,7 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -543,9 +543,9 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9"/>
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
       <c r="E5" s="1"/>

</xml_diff>

<commit_message>
cap nhat UI va Phan cong
</commit_message>
<xml_diff>
--- a/Do_An/Phân Công.xlsx
+++ b/Do_An/Phân Công.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tai lieu HK V\Android\Thunder_Team\Do_An\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tai lieu HK V\Android\DA_Android\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>MSSV_Họ Tên</t>
   </si>
@@ -61,6 +61,28 @@
   </si>
   <si>
     <t>Chưa Hoàn Thành</t>
+  </si>
+  <si>
+    <t>- Thiết kế màn hình: 
+  + Danh sách bài viết
+  + Trang cá nhân
+  + Danh sách địa danh
+  + Chi tiết địa danh
+  + Tìm kiếm
+  + Danh sách người like</t>
+  </si>
+  <si>
+    <t>- Thiết kế màn hình:
+  + Tạo đề xuất
+  + Tạo bài viết
+  + Chỉnh sửa thông tin cá nhân
+  + Đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>- Thiết kế màn hình:
+  + Đăng nhập
+  + Đăng ký tài khoản
+  + Chi tiết thông tin cá nhân</t>
   </si>
 </sst>
 </file>
@@ -119,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -142,11 +164,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,6 +238,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -463,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -547,21 +625,51 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="E7" s="1"/>
+    <row r="5" spans="1:6" ht="137.25" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="112.5" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" ht="79.5" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6">
       <c r="E8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update UI: Login + Sign up
</commit_message>
<xml_diff>
--- a/Do_An/Phân Công.xlsx
+++ b/Do_An/Phân Công.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tai lieu HK V\Android\DA_Android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tai lieu HK V\Android\Thunder_Team\Do_An\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -205,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,18 +237,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,7 +539,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -589,7 +586,7 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="14">
         <v>9</v>
       </c>
     </row>
@@ -607,7 +604,7 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" ht="22.5" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -623,19 +620,21 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="137.25" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="16">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
         <v>10</v>
       </c>
     </row>
@@ -643,25 +642,29 @@
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="79.5" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="18"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6">
       <c r="E8" s="1"/>

</xml_diff>